<commit_message>
update nodered node to support connect with uns
</commit_message>
<xml_diff>
--- a/mount/node-red/template/template-cn.xlsx
+++ b/mount/node-red/template/template-cn.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:dbsheet="http://web.wps.cn/et/2021/dbsheet">
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27945" windowHeight="12375"/>
+    <workbookView windowWidth="28800" windowHeight="12255"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -45,19 +45,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <rFont val="宋体"/>
-            <charset val="134"/>
-          </rPr>
-          <t>输入长度小于63，支持中文、字母、数字、下划线</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D1" authorId="0">
+    <comment ref="C1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -69,7 +57,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0">
+    <comment ref="D1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -87,7 +75,7 @@
             <rFont val="宋体"/>
             <charset val="134"/>
           </rPr>
-          <t>int
+          <t>integer
 long
 double
 float
@@ -97,7 +85,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0">
+    <comment ref="E1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -169,12 +157,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t>文件夹路径（必填）</t>
-  </si>
-  <si>
-    <t>文件名称（必填）</t>
+    <t>文件路径（必填）</t>
   </si>
   <si>
     <t>文件别名</t>
@@ -352,12 +337,12 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="9"/>
       <name val="宋体"/>
       <charset val="134"/>
     </font>
     <font>
-      <b/>
       <sz val="9"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -900,6 +885,13 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/customStorage/customStorage.xml><?xml version="1.0" encoding="utf-8"?>
+<customStorage xmlns="https://web.wps.cn/et/2018/main">
+  <book/>
+  <sheets/>
+</customStorage>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1152,21 +1144,21 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="3" width="21.125" customWidth="1"/>
-    <col min="4" max="4" width="20.875" customWidth="1"/>
-    <col min="5" max="5" width="24.375" customWidth="1"/>
-    <col min="6" max="6" width="32.75" customWidth="1"/>
+    <col min="1" max="2" width="21.125" customWidth="1"/>
+    <col min="3" max="3" width="20.875" customWidth="1"/>
+    <col min="4" max="4" width="24.375" customWidth="1"/>
+    <col min="5" max="5" width="32.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="28" customHeight="1" spans="1:6">
+    <row r="1" ht="28" customHeight="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1182,11 +1174,8 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
     </row>
-    <row r="2" ht="63" customHeight="1"/>
+    <row r="2" ht="24" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>